<commit_message>
Figure settings again and again
</commit_message>
<xml_diff>
--- a/output/sites/clustering with all nutrients/clust_all_nut_compo_sites.xlsx
+++ b/output/sites/clustering with all nutrients/clust_all_nut_compo_sites.xlsx
@@ -586,73 +586,73 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="E3" t="n">
-        <v>26999.6</v>
+        <v>22532.029</v>
       </c>
       <c r="F3" t="n">
-        <v>8512.157</v>
+        <v>5735.173</v>
       </c>
       <c r="G3" t="n">
-        <v>472.372</v>
+        <v>520.784</v>
       </c>
       <c r="H3" t="n">
-        <v>286.031</v>
+        <v>314.07</v>
       </c>
       <c r="I3" t="n">
-        <v>129.883</v>
+        <v>103.288</v>
       </c>
       <c r="J3" t="n">
-        <v>35.409</v>
+        <v>39.092</v>
       </c>
       <c r="K3" t="n">
-        <v>6.596</v>
+        <v>4.736</v>
       </c>
       <c r="L3" t="n">
-        <v>19597.558</v>
+        <v>12990.3</v>
       </c>
       <c r="M3" t="n">
-        <v>7724.266</v>
+        <v>4315.638</v>
       </c>
       <c r="N3" t="n">
-        <v>530.447</v>
+        <v>544.624</v>
       </c>
       <c r="O3" t="n">
-        <v>193.435</v>
+        <v>241.627</v>
       </c>
       <c r="P3" t="n">
-        <v>133.266</v>
+        <v>90.469</v>
       </c>
       <c r="Q3" t="n">
-        <v>27.356</v>
+        <v>36.215</v>
       </c>
       <c r="R3" t="n">
-        <v>6.078</v>
+        <v>4.089</v>
       </c>
       <c r="S3" t="n">
-        <v>21725.527</v>
+        <v>18970.228</v>
       </c>
       <c r="T3" t="n">
-        <v>4447.689</v>
+        <v>4804.847</v>
       </c>
       <c r="U3" t="n">
-        <v>178.353</v>
+        <v>221.217</v>
       </c>
       <c r="V3" t="n">
-        <v>226.259</v>
+        <v>210.775</v>
       </c>
       <c r="W3" t="n">
-        <v>46.697</v>
+        <v>56.17</v>
       </c>
       <c r="X3" t="n">
-        <v>19.092</v>
+        <v>16.287</v>
       </c>
       <c r="Y3" t="n">
-        <v>3.285</v>
+        <v>3.439</v>
       </c>
     </row>
     <row r="4">
@@ -663,150 +663,150 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>25.9</v>
+        <v>11.1</v>
       </c>
       <c r="E4" t="n">
-        <v>16149.785</v>
+        <v>12306.656</v>
       </c>
       <c r="F4" t="n">
-        <v>1768.053</v>
+        <v>208.404</v>
       </c>
       <c r="G4" t="n">
-        <v>589.943</v>
+        <v>205.772</v>
       </c>
       <c r="H4" t="n">
-        <v>354.126</v>
+        <v>467.651</v>
       </c>
       <c r="I4" t="n">
-        <v>65.295</v>
+        <v>15.522</v>
       </c>
       <c r="J4" t="n">
-        <v>44.353</v>
+        <v>99.452</v>
       </c>
       <c r="K4" t="n">
-        <v>2.079</v>
+        <v>0.211</v>
       </c>
       <c r="L4" t="n">
-        <v>10220.335</v>
+        <v>12601.589</v>
       </c>
       <c r="M4" t="n">
-        <v>2019.078</v>
+        <v>227.884</v>
       </c>
       <c r="N4" t="n">
-        <v>586.66</v>
+        <v>106.824</v>
       </c>
       <c r="O4" t="n">
-        <v>261.025</v>
+        <v>391.766</v>
       </c>
       <c r="P4" t="n">
-        <v>51.078</v>
+        <v>15.598</v>
       </c>
       <c r="Q4" t="n">
-        <v>44.183</v>
+        <v>103.808</v>
       </c>
       <c r="R4" t="n">
-        <v>1.798</v>
+        <v>0.25</v>
       </c>
       <c r="S4" t="n">
-        <v>13071.619</v>
+        <v>7382.222</v>
       </c>
       <c r="T4" t="n">
-        <v>823.076</v>
+        <v>52.856</v>
       </c>
       <c r="U4" t="n">
-        <v>270.736</v>
+        <v>198.361</v>
       </c>
       <c r="V4" t="n">
-        <v>196.207</v>
+        <v>215.293</v>
       </c>
       <c r="W4" t="n">
-        <v>47.746</v>
+        <v>2.808</v>
       </c>
       <c r="X4" t="n">
-        <v>10.283</v>
+        <v>29.422</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.16</v>
+        <v>0.071</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>11.1</v>
+        <v>34.5</v>
       </c>
       <c r="E5" t="n">
-        <v>12306.656</v>
+        <v>110452.318</v>
       </c>
       <c r="F5" t="n">
-        <v>208.404</v>
+        <v>305.278</v>
       </c>
       <c r="G5" t="n">
-        <v>205.772</v>
+        <v>315.733</v>
       </c>
       <c r="H5" t="n">
-        <v>467.651</v>
+        <v>27.459</v>
       </c>
       <c r="I5" t="n">
-        <v>15.522</v>
+        <v>18.822</v>
       </c>
       <c r="J5" t="n">
-        <v>99.452</v>
+        <v>9.332</v>
       </c>
       <c r="K5" t="n">
-        <v>0.211</v>
+        <v>0.479</v>
       </c>
       <c r="L5" t="n">
-        <v>12601.589</v>
+        <v>117710.229</v>
       </c>
       <c r="M5" t="n">
-        <v>227.884</v>
+        <v>288.49</v>
       </c>
       <c r="N5" t="n">
-        <v>106.824</v>
+        <v>279.906</v>
       </c>
       <c r="O5" t="n">
-        <v>391.766</v>
+        <v>19.797</v>
       </c>
       <c r="P5" t="n">
-        <v>15.598</v>
+        <v>17.859</v>
       </c>
       <c r="Q5" t="n">
-        <v>103.808</v>
+        <v>7.634</v>
       </c>
       <c r="R5" t="n">
-        <v>0.25</v>
+        <v>0.505</v>
       </c>
       <c r="S5" t="n">
-        <v>7382.222</v>
+        <v>21627.218</v>
       </c>
       <c r="T5" t="n">
-        <v>52.856</v>
+        <v>69.95</v>
       </c>
       <c r="U5" t="n">
-        <v>198.361</v>
+        <v>86.88</v>
       </c>
       <c r="V5" t="n">
-        <v>215.293</v>
+        <v>13.756</v>
       </c>
       <c r="W5" t="n">
-        <v>2.808</v>
+        <v>4.337</v>
       </c>
       <c r="X5" t="n">
-        <v>29.422</v>
+        <v>4.187</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.071</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="6">
@@ -814,76 +814,76 @@
         <v>26</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>34.5</v>
+        <v>48.3</v>
       </c>
       <c r="E6" t="n">
-        <v>110452.318</v>
+        <v>23936.879</v>
       </c>
       <c r="F6" t="n">
-        <v>305.278</v>
+        <v>6843.513</v>
       </c>
       <c r="G6" t="n">
-        <v>315.733</v>
+        <v>423.481</v>
       </c>
       <c r="H6" t="n">
-        <v>27.459</v>
+        <v>179.325</v>
       </c>
       <c r="I6" t="n">
-        <v>18.822</v>
+        <v>177.809</v>
       </c>
       <c r="J6" t="n">
-        <v>9.332</v>
+        <v>34.8</v>
       </c>
       <c r="K6" t="n">
-        <v>0.479</v>
+        <v>5.327</v>
       </c>
       <c r="L6" t="n">
-        <v>117710.229</v>
+        <v>16781.135</v>
       </c>
       <c r="M6" t="n">
-        <v>288.49</v>
+        <v>7496.46</v>
       </c>
       <c r="N6" t="n">
-        <v>279.906</v>
+        <v>345.057</v>
       </c>
       <c r="O6" t="n">
-        <v>19.797</v>
+        <v>154.624</v>
       </c>
       <c r="P6" t="n">
-        <v>17.859</v>
+        <v>175.608</v>
       </c>
       <c r="Q6" t="n">
-        <v>7.634</v>
+        <v>33.575</v>
       </c>
       <c r="R6" t="n">
-        <v>0.505</v>
+        <v>6.147</v>
       </c>
       <c r="S6" t="n">
-        <v>21627.218</v>
+        <v>16241.445</v>
       </c>
       <c r="T6" t="n">
-        <v>69.95</v>
+        <v>4475.689</v>
       </c>
       <c r="U6" t="n">
-        <v>86.88</v>
+        <v>268.038</v>
       </c>
       <c r="V6" t="n">
-        <v>13.756</v>
+        <v>123.838</v>
       </c>
       <c r="W6" t="n">
-        <v>4.337</v>
+        <v>127.96</v>
       </c>
       <c r="X6" t="n">
-        <v>4.187</v>
+        <v>20.244</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.107</v>
+        <v>3.384</v>
       </c>
     </row>
     <row r="7">
@@ -891,152 +891,75 @@
         <v>26</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>48.3</v>
+        <v>17.2</v>
       </c>
       <c r="E7" t="n">
-        <v>23936.879</v>
+        <v>19128.34</v>
       </c>
       <c r="F7" t="n">
-        <v>6843.513</v>
+        <v>266.372</v>
       </c>
       <c r="G7" t="n">
-        <v>423.481</v>
+        <v>249.043</v>
       </c>
       <c r="H7" t="n">
-        <v>179.325</v>
+        <v>75.325</v>
       </c>
       <c r="I7" t="n">
-        <v>177.809</v>
+        <v>18.2</v>
       </c>
       <c r="J7" t="n">
-        <v>34.8</v>
+        <v>26.708</v>
       </c>
       <c r="K7" t="n">
-        <v>5.327</v>
+        <v>0.399</v>
       </c>
       <c r="L7" t="n">
-        <v>16781.135</v>
+        <v>6676.001</v>
       </c>
       <c r="M7" t="n">
-        <v>7496.46</v>
+        <v>209.627</v>
       </c>
       <c r="N7" t="n">
-        <v>345.057</v>
+        <v>326.674</v>
       </c>
       <c r="O7" t="n">
-        <v>154.624</v>
+        <v>67.169</v>
       </c>
       <c r="P7" t="n">
-        <v>175.608</v>
+        <v>19.73</v>
       </c>
       <c r="Q7" t="n">
-        <v>33.575</v>
+        <v>28.549</v>
       </c>
       <c r="R7" t="n">
-        <v>6.147</v>
+        <v>0.435</v>
       </c>
       <c r="S7" t="n">
-        <v>16241.445</v>
+        <v>24845.357</v>
       </c>
       <c r="T7" t="n">
-        <v>4475.689</v>
+        <v>202.103</v>
       </c>
       <c r="U7" t="n">
-        <v>268.038</v>
+        <v>179.514</v>
       </c>
       <c r="V7" t="n">
-        <v>123.838</v>
+        <v>41.895</v>
       </c>
       <c r="W7" t="n">
-        <v>127.96</v>
+        <v>5.048</v>
       </c>
       <c r="X7" t="n">
-        <v>20.244</v>
+        <v>13.213</v>
       </c>
       <c r="Y7" t="n">
-        <v>3.384</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" t="n">
-        <v>5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>19128.34</v>
-      </c>
-      <c r="F8" t="n">
-        <v>266.372</v>
-      </c>
-      <c r="G8" t="n">
-        <v>249.043</v>
-      </c>
-      <c r="H8" t="n">
-        <v>75.325</v>
-      </c>
-      <c r="I8" t="n">
-        <v>18.2</v>
-      </c>
-      <c r="J8" t="n">
-        <v>26.708</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.399</v>
-      </c>
-      <c r="L8" t="n">
-        <v>6676.001</v>
-      </c>
-      <c r="M8" t="n">
-        <v>209.627</v>
-      </c>
-      <c r="N8" t="n">
-        <v>326.674</v>
-      </c>
-      <c r="O8" t="n">
-        <v>67.169</v>
-      </c>
-      <c r="P8" t="n">
-        <v>19.73</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>28.549</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.435</v>
-      </c>
-      <c r="S8" t="n">
-        <v>24845.357</v>
-      </c>
-      <c r="T8" t="n">
-        <v>202.103</v>
-      </c>
-      <c r="U8" t="n">
-        <v>179.514</v>
-      </c>
-      <c r="V8" t="n">
-        <v>41.895</v>
-      </c>
-      <c r="W8" t="n">
-        <v>5.048</v>
-      </c>
-      <c r="X8" t="n">
-        <v>13.213</v>
-      </c>
-      <c r="Y8" t="n">
         <v>0.233</v>
       </c>
     </row>

</xml_diff>